<commit_message>
update palm output & generate plots
</commit_message>
<xml_diff>
--- a/code/df_contra_full_left.xlsx
+++ b/code/df_contra_full_left.xlsx
@@ -13,7 +13,1072 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="639">
+  <si>
+    <t>Subs</t>
+  </si>
+  <si>
+    <t>IV-doors</t>
+  </si>
+  <si>
+    <t>IV-socialdoors</t>
+  </si>
+  <si>
+    <t>IV-ugdg</t>
+  </si>
+  <si>
+    <t>IV-mid</t>
+  </si>
+  <si>
+    <t>IV-sharedreward</t>
+  </si>
+  <si>
+    <t>V-doors</t>
+  </si>
+  <si>
+    <t>V-socialdoors</t>
+  </si>
+  <si>
+    <t>V-ugdg</t>
+  </si>
+  <si>
+    <t>V-mid</t>
+  </si>
+  <si>
+    <t>V-sharedreward</t>
+  </si>
+  <si>
+    <t>VI-doors</t>
+  </si>
+  <si>
+    <t>VI-socialdoors</t>
+  </si>
+  <si>
+    <t>VI-ugdg</t>
+  </si>
+  <si>
+    <t>VI-mid</t>
+  </si>
+  <si>
+    <t>VI-sharedreward</t>
+  </si>
+  <si>
+    <t>Crus-I-doors</t>
+  </si>
+  <si>
+    <t>Crus-I-socialdoors</t>
+  </si>
+  <si>
+    <t>Crus-I-ugdg</t>
+  </si>
+  <si>
+    <t>Crus-I-mid</t>
+  </si>
+  <si>
+    <t>Crus-I-sharedreward</t>
+  </si>
+  <si>
+    <t>Crus-II-doors</t>
+  </si>
+  <si>
+    <t>Crus-II-socialdoors</t>
+  </si>
+  <si>
+    <t>Crus-II-ugdg</t>
+  </si>
+  <si>
+    <t>Crus-II-mid</t>
+  </si>
+  <si>
+    <t>Crus-II-sharedreward</t>
+  </si>
+  <si>
+    <t>VIIb-doors</t>
+  </si>
+  <si>
+    <t>VIIb-socialdoors</t>
+  </si>
+  <si>
+    <t>VIIb-ugdg</t>
+  </si>
+  <si>
+    <t>VIIb-mid</t>
+  </si>
+  <si>
+    <t>VIIb-sharedreward</t>
+  </si>
+  <si>
+    <t>VIIIa-doors</t>
+  </si>
+  <si>
+    <t>VIIIa-socialdoors</t>
+  </si>
+  <si>
+    <t>VIIIa-ugdg</t>
+  </si>
+  <si>
+    <t>VIIIa-mid</t>
+  </si>
+  <si>
+    <t>VIIIa-sharedreward</t>
+  </si>
+  <si>
+    <t>VIIIb-doors</t>
+  </si>
+  <si>
+    <t>VIIIb-socialdoors</t>
+  </si>
+  <si>
+    <t>VIIIb-ugdg</t>
+  </si>
+  <si>
+    <t>VIIIb-mid</t>
+  </si>
+  <si>
+    <t>VIIIb-sharedreward</t>
+  </si>
+  <si>
+    <t>IX-doors</t>
+  </si>
+  <si>
+    <t>IX-socialdoors</t>
+  </si>
+  <si>
+    <t>IX-ugdg</t>
+  </si>
+  <si>
+    <t>IX-mid</t>
+  </si>
+  <si>
+    <t>IX-sharedreward</t>
+  </si>
+  <si>
+    <t>X-doors</t>
+  </si>
+  <si>
+    <t>X-socialdoors</t>
+  </si>
+  <si>
+    <t>X-ugdg</t>
+  </si>
+  <si>
+    <t>X-mid</t>
+  </si>
+  <si>
+    <t>X-sharedreward</t>
+  </si>
+  <si>
+    <t>Vermis-VI-doors</t>
+  </si>
+  <si>
+    <t>Vermis-VI-socialdoors</t>
+  </si>
+  <si>
+    <t>Vermis-VI-ugdg</t>
+  </si>
+  <si>
+    <t>Vermis-VI-mid</t>
+  </si>
+  <si>
+    <t>Vermis-VI-sharedreward</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIa-doors</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIa-socialdoors</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIa-ugdg</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIa-mid</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIa-sharedreward</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIb-doors</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIb-socialdoors</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIb-ugdg</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIb-mid</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIb-sharedreward</t>
+  </si>
+  <si>
+    <t>Vermis-IX-doors</t>
+  </si>
+  <si>
+    <t>Vermis-IX-socialdoors</t>
+  </si>
+  <si>
+    <t>Vermis-IX-ugdg</t>
+  </si>
+  <si>
+    <t>Vermis-IX-mid</t>
+  </si>
+  <si>
+    <t>Vermis-IX-sharedreward</t>
+  </si>
+  <si>
+    <t>Subs</t>
+  </si>
+  <si>
+    <t>IV-doors</t>
+  </si>
+  <si>
+    <t>IV-socialdoors</t>
+  </si>
+  <si>
+    <t>IV-ugdg</t>
+  </si>
+  <si>
+    <t>IV-mid</t>
+  </si>
+  <si>
+    <t>IV-sharedreward</t>
+  </si>
+  <si>
+    <t>V-doors</t>
+  </si>
+  <si>
+    <t>V-socialdoors</t>
+  </si>
+  <si>
+    <t>V-ugdg</t>
+  </si>
+  <si>
+    <t>V-mid</t>
+  </si>
+  <si>
+    <t>V-sharedreward</t>
+  </si>
+  <si>
+    <t>VI-doors</t>
+  </si>
+  <si>
+    <t>VI-socialdoors</t>
+  </si>
+  <si>
+    <t>VI-ugdg</t>
+  </si>
+  <si>
+    <t>VI-mid</t>
+  </si>
+  <si>
+    <t>VI-sharedreward</t>
+  </si>
+  <si>
+    <t>Crus-I-doors</t>
+  </si>
+  <si>
+    <t>Crus-I-socialdoors</t>
+  </si>
+  <si>
+    <t>Crus-I-ugdg</t>
+  </si>
+  <si>
+    <t>Crus-I-mid</t>
+  </si>
+  <si>
+    <t>Crus-I-sharedreward</t>
+  </si>
+  <si>
+    <t>Crus-II-doors</t>
+  </si>
+  <si>
+    <t>Crus-II-socialdoors</t>
+  </si>
+  <si>
+    <t>Crus-II-ugdg</t>
+  </si>
+  <si>
+    <t>Crus-II-mid</t>
+  </si>
+  <si>
+    <t>Crus-II-sharedreward</t>
+  </si>
+  <si>
+    <t>VIIb-doors</t>
+  </si>
+  <si>
+    <t>VIIb-socialdoors</t>
+  </si>
+  <si>
+    <t>VIIb-ugdg</t>
+  </si>
+  <si>
+    <t>VIIb-mid</t>
+  </si>
+  <si>
+    <t>VIIb-sharedreward</t>
+  </si>
+  <si>
+    <t>VIIIa-doors</t>
+  </si>
+  <si>
+    <t>VIIIa-socialdoors</t>
+  </si>
+  <si>
+    <t>VIIIa-ugdg</t>
+  </si>
+  <si>
+    <t>VIIIa-mid</t>
+  </si>
+  <si>
+    <t>VIIIa-sharedreward</t>
+  </si>
+  <si>
+    <t>VIIIb-doors</t>
+  </si>
+  <si>
+    <t>VIIIb-socialdoors</t>
+  </si>
+  <si>
+    <t>VIIIb-ugdg</t>
+  </si>
+  <si>
+    <t>VIIIb-mid</t>
+  </si>
+  <si>
+    <t>VIIIb-sharedreward</t>
+  </si>
+  <si>
+    <t>IX-doors</t>
+  </si>
+  <si>
+    <t>IX-socialdoors</t>
+  </si>
+  <si>
+    <t>IX-ugdg</t>
+  </si>
+  <si>
+    <t>IX-mid</t>
+  </si>
+  <si>
+    <t>IX-sharedreward</t>
+  </si>
+  <si>
+    <t>X-doors</t>
+  </si>
+  <si>
+    <t>X-socialdoors</t>
+  </si>
+  <si>
+    <t>X-ugdg</t>
+  </si>
+  <si>
+    <t>X-mid</t>
+  </si>
+  <si>
+    <t>X-sharedreward</t>
+  </si>
+  <si>
+    <t>Vermis-VI-doors</t>
+  </si>
+  <si>
+    <t>Vermis-VI-socialdoors</t>
+  </si>
+  <si>
+    <t>Vermis-VI-ugdg</t>
+  </si>
+  <si>
+    <t>Vermis-VI-mid</t>
+  </si>
+  <si>
+    <t>Vermis-VI-sharedreward</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIa-doors</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIa-socialdoors</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIa-ugdg</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIa-mid</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIa-sharedreward</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIb-doors</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIb-socialdoors</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIb-ugdg</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIb-mid</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIb-sharedreward</t>
+  </si>
+  <si>
+    <t>Vermis-IX-doors</t>
+  </si>
+  <si>
+    <t>Vermis-IX-socialdoors</t>
+  </si>
+  <si>
+    <t>Vermis-IX-ugdg</t>
+  </si>
+  <si>
+    <t>Vermis-IX-mid</t>
+  </si>
+  <si>
+    <t>Vermis-IX-sharedreward</t>
+  </si>
+  <si>
+    <t>Subs</t>
+  </si>
+  <si>
+    <t>IV-doors</t>
+  </si>
+  <si>
+    <t>IV-socialdoors</t>
+  </si>
+  <si>
+    <t>IV-ugdg</t>
+  </si>
+  <si>
+    <t>IV-mid</t>
+  </si>
+  <si>
+    <t>IV-sharedreward</t>
+  </si>
+  <si>
+    <t>V-doors</t>
+  </si>
+  <si>
+    <t>V-socialdoors</t>
+  </si>
+  <si>
+    <t>V-ugdg</t>
+  </si>
+  <si>
+    <t>V-mid</t>
+  </si>
+  <si>
+    <t>V-sharedreward</t>
+  </si>
+  <si>
+    <t>VI-doors</t>
+  </si>
+  <si>
+    <t>VI-socialdoors</t>
+  </si>
+  <si>
+    <t>VI-ugdg</t>
+  </si>
+  <si>
+    <t>VI-mid</t>
+  </si>
+  <si>
+    <t>VI-sharedreward</t>
+  </si>
+  <si>
+    <t>Crus-I-doors</t>
+  </si>
+  <si>
+    <t>Crus-I-socialdoors</t>
+  </si>
+  <si>
+    <t>Crus-I-ugdg</t>
+  </si>
+  <si>
+    <t>Crus-I-mid</t>
+  </si>
+  <si>
+    <t>Crus-I-sharedreward</t>
+  </si>
+  <si>
+    <t>Crus-II-doors</t>
+  </si>
+  <si>
+    <t>Crus-II-socialdoors</t>
+  </si>
+  <si>
+    <t>Crus-II-ugdg</t>
+  </si>
+  <si>
+    <t>Crus-II-mid</t>
+  </si>
+  <si>
+    <t>Crus-II-sharedreward</t>
+  </si>
+  <si>
+    <t>VIIb-doors</t>
+  </si>
+  <si>
+    <t>VIIb-socialdoors</t>
+  </si>
+  <si>
+    <t>VIIb-ugdg</t>
+  </si>
+  <si>
+    <t>VIIb-mid</t>
+  </si>
+  <si>
+    <t>VIIb-sharedreward</t>
+  </si>
+  <si>
+    <t>VIIIa-doors</t>
+  </si>
+  <si>
+    <t>VIIIa-socialdoors</t>
+  </si>
+  <si>
+    <t>VIIIa-ugdg</t>
+  </si>
+  <si>
+    <t>VIIIa-mid</t>
+  </si>
+  <si>
+    <t>VIIIa-sharedreward</t>
+  </si>
+  <si>
+    <t>VIIIb-doors</t>
+  </si>
+  <si>
+    <t>VIIIb-socialdoors</t>
+  </si>
+  <si>
+    <t>VIIIb-ugdg</t>
+  </si>
+  <si>
+    <t>VIIIb-mid</t>
+  </si>
+  <si>
+    <t>VIIIb-sharedreward</t>
+  </si>
+  <si>
+    <t>IX-doors</t>
+  </si>
+  <si>
+    <t>IX-socialdoors</t>
+  </si>
+  <si>
+    <t>IX-ugdg</t>
+  </si>
+  <si>
+    <t>IX-mid</t>
+  </si>
+  <si>
+    <t>IX-sharedreward</t>
+  </si>
+  <si>
+    <t>X-doors</t>
+  </si>
+  <si>
+    <t>X-socialdoors</t>
+  </si>
+  <si>
+    <t>X-ugdg</t>
+  </si>
+  <si>
+    <t>X-mid</t>
+  </si>
+  <si>
+    <t>X-sharedreward</t>
+  </si>
+  <si>
+    <t>Vermis-VI-doors</t>
+  </si>
+  <si>
+    <t>Vermis-VI-socialdoors</t>
+  </si>
+  <si>
+    <t>Vermis-VI-ugdg</t>
+  </si>
+  <si>
+    <t>Vermis-VI-mid</t>
+  </si>
+  <si>
+    <t>Vermis-VI-sharedreward</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIa-doors</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIa-socialdoors</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIa-ugdg</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIa-mid</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIa-sharedreward</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIb-doors</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIb-socialdoors</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIb-ugdg</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIb-mid</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIb-sharedreward</t>
+  </si>
+  <si>
+    <t>Vermis-IX-doors</t>
+  </si>
+  <si>
+    <t>Vermis-IX-socialdoors</t>
+  </si>
+  <si>
+    <t>Vermis-IX-ugdg</t>
+  </si>
+  <si>
+    <t>Vermis-IX-mid</t>
+  </si>
+  <si>
+    <t>Vermis-IX-sharedreward</t>
+  </si>
+  <si>
+    <t>Subs</t>
+  </si>
+  <si>
+    <t>IV-doors</t>
+  </si>
+  <si>
+    <t>IV-socialdoors</t>
+  </si>
+  <si>
+    <t>IV-ugdg</t>
+  </si>
+  <si>
+    <t>IV-mid</t>
+  </si>
+  <si>
+    <t>IV-sharedreward</t>
+  </si>
+  <si>
+    <t>V-doors</t>
+  </si>
+  <si>
+    <t>V-socialdoors</t>
+  </si>
+  <si>
+    <t>V-ugdg</t>
+  </si>
+  <si>
+    <t>V-mid</t>
+  </si>
+  <si>
+    <t>V-sharedreward</t>
+  </si>
+  <si>
+    <t>VI-doors</t>
+  </si>
+  <si>
+    <t>VI-socialdoors</t>
+  </si>
+  <si>
+    <t>VI-ugdg</t>
+  </si>
+  <si>
+    <t>VI-mid</t>
+  </si>
+  <si>
+    <t>VI-sharedreward</t>
+  </si>
+  <si>
+    <t>Crus-I-doors</t>
+  </si>
+  <si>
+    <t>Crus-I-socialdoors</t>
+  </si>
+  <si>
+    <t>Crus-I-ugdg</t>
+  </si>
+  <si>
+    <t>Crus-I-mid</t>
+  </si>
+  <si>
+    <t>Crus-I-sharedreward</t>
+  </si>
+  <si>
+    <t>Crus-II-doors</t>
+  </si>
+  <si>
+    <t>Crus-II-socialdoors</t>
+  </si>
+  <si>
+    <t>Crus-II-ugdg</t>
+  </si>
+  <si>
+    <t>Crus-II-mid</t>
+  </si>
+  <si>
+    <t>Crus-II-sharedreward</t>
+  </si>
+  <si>
+    <t>VIIb-doors</t>
+  </si>
+  <si>
+    <t>VIIb-socialdoors</t>
+  </si>
+  <si>
+    <t>VIIb-ugdg</t>
+  </si>
+  <si>
+    <t>VIIb-mid</t>
+  </si>
+  <si>
+    <t>VIIb-sharedreward</t>
+  </si>
+  <si>
+    <t>VIIIa-doors</t>
+  </si>
+  <si>
+    <t>VIIIa-socialdoors</t>
+  </si>
+  <si>
+    <t>VIIIa-ugdg</t>
+  </si>
+  <si>
+    <t>VIIIa-mid</t>
+  </si>
+  <si>
+    <t>VIIIa-sharedreward</t>
+  </si>
+  <si>
+    <t>VIIIb-doors</t>
+  </si>
+  <si>
+    <t>VIIIb-socialdoors</t>
+  </si>
+  <si>
+    <t>VIIIb-ugdg</t>
+  </si>
+  <si>
+    <t>VIIIb-mid</t>
+  </si>
+  <si>
+    <t>VIIIb-sharedreward</t>
+  </si>
+  <si>
+    <t>IX-doors</t>
+  </si>
+  <si>
+    <t>IX-socialdoors</t>
+  </si>
+  <si>
+    <t>IX-ugdg</t>
+  </si>
+  <si>
+    <t>IX-mid</t>
+  </si>
+  <si>
+    <t>IX-sharedreward</t>
+  </si>
+  <si>
+    <t>X-doors</t>
+  </si>
+  <si>
+    <t>X-socialdoors</t>
+  </si>
+  <si>
+    <t>X-ugdg</t>
+  </si>
+  <si>
+    <t>X-mid</t>
+  </si>
+  <si>
+    <t>X-sharedreward</t>
+  </si>
+  <si>
+    <t>Vermis-VI-doors</t>
+  </si>
+  <si>
+    <t>Vermis-VI-socialdoors</t>
+  </si>
+  <si>
+    <t>Vermis-VI-ugdg</t>
+  </si>
+  <si>
+    <t>Vermis-VI-mid</t>
+  </si>
+  <si>
+    <t>Vermis-VI-sharedreward</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIa-doors</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIa-socialdoors</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIa-ugdg</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIa-mid</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIa-sharedreward</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIb-doors</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIb-socialdoors</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIb-ugdg</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIb-mid</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIb-sharedreward</t>
+  </si>
+  <si>
+    <t>Vermis-IX-doors</t>
+  </si>
+  <si>
+    <t>Vermis-IX-socialdoors</t>
+  </si>
+  <si>
+    <t>Vermis-IX-ugdg</t>
+  </si>
+  <si>
+    <t>Vermis-IX-mid</t>
+  </si>
+  <si>
+    <t>Vermis-IX-sharedreward</t>
+  </si>
+  <si>
+    <t>Subs</t>
+  </si>
+  <si>
+    <t>IV-doors</t>
+  </si>
+  <si>
+    <t>IV-socialdoors</t>
+  </si>
+  <si>
+    <t>IV-ugdg</t>
+  </si>
+  <si>
+    <t>IV-mid</t>
+  </si>
+  <si>
+    <t>IV-sharedreward</t>
+  </si>
+  <si>
+    <t>V-doors</t>
+  </si>
+  <si>
+    <t>V-socialdoors</t>
+  </si>
+  <si>
+    <t>V-ugdg</t>
+  </si>
+  <si>
+    <t>V-mid</t>
+  </si>
+  <si>
+    <t>V-sharedreward</t>
+  </si>
+  <si>
+    <t>VI-doors</t>
+  </si>
+  <si>
+    <t>VI-socialdoors</t>
+  </si>
+  <si>
+    <t>VI-ugdg</t>
+  </si>
+  <si>
+    <t>VI-mid</t>
+  </si>
+  <si>
+    <t>VI-sharedreward</t>
+  </si>
+  <si>
+    <t>Crus-I-doors</t>
+  </si>
+  <si>
+    <t>Crus-I-socialdoors</t>
+  </si>
+  <si>
+    <t>Crus-I-ugdg</t>
+  </si>
+  <si>
+    <t>Crus-I-mid</t>
+  </si>
+  <si>
+    <t>Crus-I-sharedreward</t>
+  </si>
+  <si>
+    <t>Crus-II-doors</t>
+  </si>
+  <si>
+    <t>Crus-II-socialdoors</t>
+  </si>
+  <si>
+    <t>Crus-II-ugdg</t>
+  </si>
+  <si>
+    <t>Crus-II-mid</t>
+  </si>
+  <si>
+    <t>Crus-II-sharedreward</t>
+  </si>
+  <si>
+    <t>VIIb-doors</t>
+  </si>
+  <si>
+    <t>VIIb-socialdoors</t>
+  </si>
+  <si>
+    <t>VIIb-ugdg</t>
+  </si>
+  <si>
+    <t>VIIb-mid</t>
+  </si>
+  <si>
+    <t>VIIb-sharedreward</t>
+  </si>
+  <si>
+    <t>VIIIa-doors</t>
+  </si>
+  <si>
+    <t>VIIIa-socialdoors</t>
+  </si>
+  <si>
+    <t>VIIIa-ugdg</t>
+  </si>
+  <si>
+    <t>VIIIa-mid</t>
+  </si>
+  <si>
+    <t>VIIIa-sharedreward</t>
+  </si>
+  <si>
+    <t>VIIIb-doors</t>
+  </si>
+  <si>
+    <t>VIIIb-socialdoors</t>
+  </si>
+  <si>
+    <t>VIIIb-ugdg</t>
+  </si>
+  <si>
+    <t>VIIIb-mid</t>
+  </si>
+  <si>
+    <t>VIIIb-sharedreward</t>
+  </si>
+  <si>
+    <t>IX-doors</t>
+  </si>
+  <si>
+    <t>IX-socialdoors</t>
+  </si>
+  <si>
+    <t>IX-ugdg</t>
+  </si>
+  <si>
+    <t>IX-mid</t>
+  </si>
+  <si>
+    <t>IX-sharedreward</t>
+  </si>
+  <si>
+    <t>X-doors</t>
+  </si>
+  <si>
+    <t>X-socialdoors</t>
+  </si>
+  <si>
+    <t>X-ugdg</t>
+  </si>
+  <si>
+    <t>X-mid</t>
+  </si>
+  <si>
+    <t>X-sharedreward</t>
+  </si>
+  <si>
+    <t>Vermis-VI-doors</t>
+  </si>
+  <si>
+    <t>Vermis-VI-socialdoors</t>
+  </si>
+  <si>
+    <t>Vermis-VI-ugdg</t>
+  </si>
+  <si>
+    <t>Vermis-VI-mid</t>
+  </si>
+  <si>
+    <t>Vermis-VI-sharedreward</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIa-doors</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIa-socialdoors</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIa-ugdg</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIa-mid</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIa-sharedreward</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIb-doors</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIb-socialdoors</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIb-ugdg</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIb-mid</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIb-sharedreward</t>
+  </si>
+  <si>
+    <t>Vermis-IX-doors</t>
+  </si>
+  <si>
+    <t>Vermis-IX-socialdoors</t>
+  </si>
+  <si>
+    <t>Vermis-IX-ugdg</t>
+  </si>
+  <si>
+    <t>Vermis-IX-mid</t>
+  </si>
+  <si>
+    <t>Vermis-IX-sharedreward</t>
+  </si>
   <si>
     <t>Subs</t>
   </si>
@@ -988,217 +2053,217 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>213</v>
+        <v>568</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>214</v>
+        <v>569</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>215</v>
+        <v>570</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>216</v>
+        <v>571</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>217</v>
+        <v>572</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>218</v>
+        <v>573</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>219</v>
+        <v>574</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>220</v>
+        <v>575</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>221</v>
+        <v>576</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>222</v>
+        <v>577</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>223</v>
+        <v>578</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>224</v>
+        <v>579</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>225</v>
+        <v>580</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>226</v>
+        <v>581</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>227</v>
+        <v>582</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>228</v>
+        <v>583</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>229</v>
+        <v>584</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>230</v>
+        <v>585</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>231</v>
+        <v>586</v>
       </c>
       <c r="T1" s="0" t="s">
-        <v>232</v>
+        <v>587</v>
       </c>
       <c r="U1" s="0" t="s">
-        <v>233</v>
+        <v>588</v>
       </c>
       <c r="V1" s="0" t="s">
-        <v>234</v>
+        <v>589</v>
       </c>
       <c r="W1" s="0" t="s">
-        <v>235</v>
+        <v>590</v>
       </c>
       <c r="X1" s="0" t="s">
-        <v>236</v>
+        <v>591</v>
       </c>
       <c r="Y1" s="0" t="s">
-        <v>237</v>
+        <v>592</v>
       </c>
       <c r="Z1" s="0" t="s">
-        <v>238</v>
+        <v>593</v>
       </c>
       <c r="AA1" s="0" t="s">
-        <v>239</v>
+        <v>594</v>
       </c>
       <c r="AB1" s="0" t="s">
-        <v>240</v>
+        <v>595</v>
       </c>
       <c r="AC1" s="0" t="s">
-        <v>241</v>
+        <v>596</v>
       </c>
       <c r="AD1" s="0" t="s">
-        <v>242</v>
+        <v>597</v>
       </c>
       <c r="AE1" s="0" t="s">
-        <v>243</v>
+        <v>598</v>
       </c>
       <c r="AF1" s="0" t="s">
-        <v>244</v>
+        <v>599</v>
       </c>
       <c r="AG1" s="0" t="s">
-        <v>245</v>
+        <v>600</v>
       </c>
       <c r="AH1" s="0" t="s">
-        <v>246</v>
+        <v>601</v>
       </c>
       <c r="AI1" s="0" t="s">
-        <v>247</v>
+        <v>602</v>
       </c>
       <c r="AJ1" s="0" t="s">
-        <v>248</v>
+        <v>603</v>
       </c>
       <c r="AK1" s="0" t="s">
-        <v>249</v>
+        <v>604</v>
       </c>
       <c r="AL1" s="0" t="s">
-        <v>250</v>
+        <v>605</v>
       </c>
       <c r="AM1" s="0" t="s">
-        <v>251</v>
+        <v>606</v>
       </c>
       <c r="AN1" s="0" t="s">
-        <v>252</v>
+        <v>607</v>
       </c>
       <c r="AO1" s="0" t="s">
-        <v>253</v>
+        <v>608</v>
       </c>
       <c r="AP1" s="0" t="s">
-        <v>254</v>
+        <v>609</v>
       </c>
       <c r="AQ1" s="0" t="s">
-        <v>255</v>
+        <v>610</v>
       </c>
       <c r="AR1" s="0" t="s">
-        <v>256</v>
+        <v>611</v>
       </c>
       <c r="AS1" s="0" t="s">
-        <v>257</v>
+        <v>612</v>
       </c>
       <c r="AT1" s="0" t="s">
-        <v>258</v>
+        <v>613</v>
       </c>
       <c r="AU1" s="0" t="s">
-        <v>259</v>
+        <v>614</v>
       </c>
       <c r="AV1" s="0" t="s">
-        <v>260</v>
+        <v>615</v>
       </c>
       <c r="AW1" s="0" t="s">
-        <v>261</v>
+        <v>616</v>
       </c>
       <c r="AX1" s="0" t="s">
-        <v>262</v>
+        <v>617</v>
       </c>
       <c r="AY1" s="0" t="s">
-        <v>263</v>
+        <v>618</v>
       </c>
       <c r="AZ1" s="0" t="s">
-        <v>264</v>
+        <v>619</v>
       </c>
       <c r="BA1" s="0" t="s">
-        <v>265</v>
+        <v>620</v>
       </c>
       <c r="BB1" s="0" t="s">
-        <v>266</v>
+        <v>621</v>
       </c>
       <c r="BC1" s="0" t="s">
-        <v>267</v>
+        <v>622</v>
       </c>
       <c r="BD1" s="0" t="s">
-        <v>268</v>
+        <v>623</v>
       </c>
       <c r="BE1" s="0" t="s">
-        <v>269</v>
+        <v>624</v>
       </c>
       <c r="BF1" s="0" t="s">
-        <v>270</v>
+        <v>625</v>
       </c>
       <c r="BG1" s="0" t="s">
-        <v>271</v>
+        <v>626</v>
       </c>
       <c r="BH1" s="0" t="s">
-        <v>272</v>
+        <v>627</v>
       </c>
       <c r="BI1" s="0" t="s">
-        <v>273</v>
+        <v>628</v>
       </c>
       <c r="BJ1" s="0" t="s">
-        <v>274</v>
+        <v>629</v>
       </c>
       <c r="BK1" s="0" t="s">
-        <v>275</v>
+        <v>630</v>
       </c>
       <c r="BL1" s="0" t="s">
-        <v>276</v>
+        <v>631</v>
       </c>
       <c r="BM1" s="0" t="s">
-        <v>277</v>
+        <v>632</v>
       </c>
       <c r="BN1" s="0" t="s">
-        <v>278</v>
+        <v>633</v>
       </c>
       <c r="BO1" s="0" t="s">
-        <v>279</v>
+        <v>634</v>
       </c>
       <c r="BP1" s="0" t="s">
-        <v>280</v>
+        <v>635</v>
       </c>
       <c r="BQ1" s="0" t="s">
-        <v>281</v>
+        <v>636</v>
       </c>
       <c r="BR1" s="0" t="s">
-        <v>282</v>
+        <v>637</v>
       </c>
       <c r="BS1" s="0" t="s">
-        <v>283</v>
+        <v>638</v>
       </c>
     </row>
     <row r="2">

</xml_diff>